<commit_message>
updated report, code mostly the same
</commit_message>
<xml_diff>
--- a/Top20.xlsx
+++ b/Top20.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\Desktop\MQP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96329F4-9C75-4EAB-AC80-6F41854A783C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BF207E-9216-4907-9266-D6B2728E6DE4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19152" windowHeight="6792" xr2:uid="{4C0D6702-A591-40D8-AFDA-9EA5D9EF5C9D}"/>
   </bookViews>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -294,7 +295,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -606,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D11B3A21-1AC3-4EEE-A272-A76B46F8C548}">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A21"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -645,7 +657,7 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>19</v>
@@ -674,7 +686,7 @@
     </row>
     <row r="3" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
@@ -703,7 +715,7 @@
     </row>
     <row r="4" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -732,7 +744,7 @@
     </row>
     <row r="5" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>2</v>
@@ -761,7 +773,7 @@
     </row>
     <row r="6" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>3</v>
@@ -790,7 +802,7 @@
     </row>
     <row r="7" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>4</v>
@@ -819,7 +831,7 @@
     </row>
     <row r="8" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>5</v>
@@ -848,7 +860,7 @@
     </row>
     <row r="9" spans="1:19" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>6</v>
@@ -877,7 +889,7 @@
     </row>
     <row r="10" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>7</v>
@@ -906,7 +918,7 @@
     </row>
     <row r="11" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>8</v>
@@ -935,7 +947,7 @@
     </row>
     <row r="12" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>9</v>
@@ -964,7 +976,7 @@
     </row>
     <row r="13" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>10</v>
@@ -993,7 +1005,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>11</v>
@@ -1022,7 +1034,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>12</v>
@@ -1051,7 +1063,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>13</v>
@@ -1080,7 +1092,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>14</v>
@@ -1109,7 +1121,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>15</v>
@@ -1138,7 +1150,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>16</v>
@@ -1167,7 +1179,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>17</v>
@@ -1196,7 +1208,7 @@
     </row>
     <row r="21" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>18</v>
@@ -1225,6 +1237,9 @@
     </row>
   </sheetData>
   <dataConsolidate/>
+  <conditionalFormatting sqref="B2:G21">
+    <cfRule type="uniqueValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>